<commit_message>
excel list 및 qty 수정
</commit_message>
<xml_diff>
--- a/intranet/src/main/resources/templates/excelFile/BookingConfirmation.xlsx
+++ b/intranet/src/main/resources/templates/excelFile/BookingConfirmation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\002\intranet\src\main\resources\templates\excelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5360330-0EFF-4D03-9957-429729BB899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6977DE8A-8C5B-48F1-9E43-738E995AD9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EAC743BB-C5B5-324B-BEB8-1702D9A24536}"/>
   </bookViews>
@@ -329,6 +329,9 @@
     <xf numFmtId="180" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,9 +343,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="119" zoomScaleNormal="176" zoomScaleSheetLayoutView="119" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="119" zoomScaleNormal="176" zoomScaleSheetLayoutView="119" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
@@ -1047,10 +1047,10 @@
     <row r="9" spans="1:5" ht="30">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
@@ -1094,10 +1094,7 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
@@ -1122,10 +1119,7 @@
       <c r="C18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D18" s="11"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
@@ -1134,10 +1128,7 @@
       <c r="C19" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
@@ -1146,10 +1137,7 @@
       <c r="C20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="13" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
@@ -1158,10 +1146,7 @@
       <c r="C21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D21" s="14"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
@@ -1170,10 +1155,7 @@
       <c r="C22" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="16" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D22" s="16"/>
       <c r="E22" s="1"/>
       <c r="J22" s="8"/>
     </row>
@@ -1181,10 +1163,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="15" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D23" s="15"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
@@ -1193,20 +1172,14 @@
       <c r="C24" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D24" s="22"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="19"/>
-      <c r="D25" s="14" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D25" s="14"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1">
@@ -1226,10 +1199,7 @@
       <c r="C27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="11" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D27" s="11"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1">
@@ -1249,10 +1219,7 @@
       <c r="C29" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D29" s="17"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1">
@@ -1261,7 +1228,7 @@
       <c r="C30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="1"/>
@@ -1270,7 +1237,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="19"/>
-      <c r="D31" s="24"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1">
@@ -1290,10 +1257,7 @@
       <c r="C33" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D33" s="17"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1">
@@ -1302,69 +1266,69 @@
       <c r="C34" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="24"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="24"/>
+      <c r="D35" s="25"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="25"/>
+      <c r="D36" s="26"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="25"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="26"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="18"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="26"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="15"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="26"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="15"/>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="26"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="15"/>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="26"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="15"/>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="26"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="10"/>
       <c r="E43" s="1"/>
     </row>
@@ -1378,24 +1342,24 @@
     <row r="45" spans="1:5" ht="15" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="24"/>
+      <c r="D45" s="25"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5">
@@ -1411,10 +1375,7 @@
       <c r="C49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D49" s="4"/>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5">
@@ -1478,10 +1439,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="27" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="D57" s="23"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5">

</xml_diff>